<commit_message>
✨ Change the inetum threshold (#1373)
Parent issue: https://github.com/sequentech/meta/issues/4833

---------

Co-authored-by: Eduardo Robles <edu@sequentech.io>
Co-authored-by: Félix Robles <felix@sequentech.io>
</commit_message>
<xml_diff>
--- a/packages/windmill/external-bin/janitor/17-12-2024-parameters-reports.xlsx
+++ b/packages/windmill/external-bin/janitor/17-12-2024-parameters-reports.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="243">
   <si>
     <t>name</t>
   </si>
@@ -29,36 +29,6 @@
   </si>
   <si>
     <t>intermediate_cas</t>
-  </si>
-  <si>
-    <t>philis_id_inetum_min_value_documental_score</t>
-  </si>
-  <si>
-    <t>philis_id_inetum_min_value_facial_score</t>
-  </si>
-  <si>
-    <t>seaman_book_inetum_min_value_val_campos_criticos_score</t>
-  </si>
-  <si>
-    <t>seaman_book_inetum_min_value_facial_score</t>
-  </si>
-  <si>
-    <t>passport_inetum_min_value_val_campos_criticos_score</t>
-  </si>
-  <si>
-    <t>passport_inetum_min_value_facial_score</t>
-  </si>
-  <si>
-    <t>driver_license_inetum_min_value_val_campos_criticos_score</t>
-  </si>
-  <si>
-    <t>driver_license_inetum_min_value_facial_score</t>
-  </si>
-  <si>
-    <t>ibp_inetum_min_value_val_campos_criticos_score</t>
-  </si>
-  <si>
-    <t>ibp_inetum_min_value_facial_score</t>
   </si>
   <si>
     <t>3 Jan Test preparations</t>
@@ -396,6 +366,45 @@
   </si>
   <si>
     <t>Hello {{{user.first_name}}} {{{user.last_name}}}!&lt;br&gt;&lt;br&gt;Your application to vote online has been rejected.&lt;br&gt;&lt;br&gt;&lt;br&gt;&lt;br&gt;Regards,&lt;br&gt;&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_philis_id_documental_score</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_philis_id_facial_score</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_seaman_book_val_campos_criticos_score</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_seaman_book_facial_score</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_passport_val_campos_criticos_score</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_passport_facial_score</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_driver_license_val_campos_criticos_score</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_driver_license_facial_score</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_ibp_val_campos_criticos_score</t>
+  </si>
+  <si>
+    <t>keycloak_inetum_min_value_ibp_facial_score</t>
   </si>
   <si>
     <t>username</t>
@@ -1084,7 +1093,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1187,11 +1196,17 @@
     <xf borderId="1" fillId="3" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -1480,36 +1495,16 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="3"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
@@ -1525,47 +1520,27 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
-      <c r="E2" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="F2" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="G2" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="H2" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="I2" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="J2" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="K2" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="L2" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="M2" s="11">
-        <v>50.0</v>
-      </c>
-      <c r="N2" s="11">
-        <v>50.0</v>
-      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
@@ -8497,31 +8472,31 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
@@ -8543,14 +8518,14 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="8" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E2" s="16" t="b">
         <v>0</v>
@@ -8579,14 +8554,14 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="18" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E3" s="19" t="b">
         <v>0</v>
@@ -8594,7 +8569,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="21"/>
       <c r="H3" s="22" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="7"/>
@@ -8617,14 +8592,14 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="18" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E4" s="19" t="b">
         <v>0</v>
@@ -8653,14 +8628,14 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="18" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E5" s="19" t="b">
         <v>0</v>
@@ -8690,20 +8665,20 @@
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="13"/>
       <c r="B6" s="18" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="18" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E6" s="19" t="b">
         <v>1</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="13"/>
@@ -15527,19 +15502,19 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -15568,16 +15543,16 @@
         <v>9.0170001E7</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -15606,16 +15581,16 @@
         <v>9.3020001E7</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -15644,16 +15619,16 @@
         <v>9.2010012E7</v>
       </c>
       <c r="B4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>44</v>
-      </c>
       <c r="D4" s="18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -15682,16 +15657,16 @@
         <v>9.1070075E7</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -15720,16 +15695,16 @@
         <v>9.1070001E7</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -22554,13 +22529,13 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -22588,13 +22563,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -22623,10 +22598,10 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="31" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
@@ -29537,13 +29512,13 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="33" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -29571,13 +29546,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>63</v>
+      <c r="C2" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -29605,13 +29580,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
@@ -29639,13 +29614,13 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
@@ -29673,13 +29648,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -29707,13 +29682,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -29741,13 +29716,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
-      <c r="C7" s="35" t="s">
-        <v>74</v>
+      <c r="C7" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -29775,13 +29750,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -29809,13 +29784,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -29843,13 +29818,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -29877,13 +29852,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
-      <c r="C11" s="35" t="s">
-        <v>82</v>
+      <c r="C11" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -29912,10 +29887,10 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="13"/>
       <c r="B12" s="18" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -29941,66 +29916,38 @@
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-      <c r="Z13" s="7"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-      <c r="Z14" s="7"/>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
+      <c r="A15" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>77</v>
+      </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -30026,9 +29973,15 @@
       <c r="Z15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>77</v>
+      </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -30054,9 +30007,15 @@
       <c r="Z16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>77</v>
+      </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -30082,9 +30041,15 @@
       <c r="Z17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>77</v>
+      </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -30110,9 +30075,15 @@
       <c r="Z18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>84</v>
+      </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -30138,9 +30109,15 @@
       <c r="Z19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>77</v>
+      </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -30165,10 +30142,16 @@
       <c r="Y20" s="7"/>
       <c r="Z20" s="7"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
+    <row r="21">
+      <c r="A21" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>77</v>
+      </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -30193,10 +30176,16 @@
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+    <row r="22">
+      <c r="A22" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>77</v>
+      </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -35765,8 +35754,62 @@
       <c r="Y220" s="7"/>
       <c r="Z220" s="7"/>
     </row>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1">
+      <c r="A221" s="7"/>
+      <c r="B221" s="7"/>
+      <c r="C221" s="7"/>
+      <c r="D221" s="7"/>
+      <c r="E221" s="7"/>
+      <c r="F221" s="7"/>
+      <c r="G221" s="7"/>
+      <c r="H221" s="7"/>
+      <c r="I221" s="7"/>
+      <c r="J221" s="7"/>
+      <c r="K221" s="7"/>
+      <c r="L221" s="7"/>
+      <c r="M221" s="7"/>
+      <c r="N221" s="7"/>
+      <c r="O221" s="7"/>
+      <c r="P221" s="7"/>
+      <c r="Q221" s="7"/>
+      <c r="R221" s="7"/>
+      <c r="S221" s="7"/>
+      <c r="T221" s="7"/>
+      <c r="U221" s="7"/>
+      <c r="V221" s="7"/>
+      <c r="W221" s="7"/>
+      <c r="X221" s="7"/>
+      <c r="Y221" s="7"/>
+      <c r="Z221" s="7"/>
+    </row>
+    <row r="222" ht="15.75" customHeight="1">
+      <c r="A222" s="7"/>
+      <c r="B222" s="7"/>
+      <c r="C222" s="7"/>
+      <c r="D222" s="7"/>
+      <c r="E222" s="7"/>
+      <c r="F222" s="7"/>
+      <c r="G222" s="7"/>
+      <c r="H222" s="7"/>
+      <c r="I222" s="7"/>
+      <c r="J222" s="7"/>
+      <c r="K222" s="7"/>
+      <c r="L222" s="7"/>
+      <c r="M222" s="7"/>
+      <c r="N222" s="7"/>
+      <c r="O222" s="7"/>
+      <c r="P222" s="7"/>
+      <c r="Q222" s="7"/>
+      <c r="R222" s="7"/>
+      <c r="S222" s="7"/>
+      <c r="T222" s="7"/>
+      <c r="U222" s="7"/>
+      <c r="V222" s="7"/>
+      <c r="W222" s="7"/>
+      <c r="X222" s="7"/>
+      <c r="Y222" s="7"/>
+      <c r="Z222" s="7"/>
+    </row>
     <row r="223" ht="15.75" customHeight="1"/>
     <row r="224" ht="15.75" customHeight="1"/>
     <row r="225" ht="15.75" customHeight="1"/>
@@ -36545,6 +36588,8 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="1.0" footer="0.0" header="0.0" left="1.0" right="1.0" top="1.0"/>
@@ -36573,22 +36618,22 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -36613,22 +36658,22 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C2" s="12" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -43566,16 +43611,16 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -43601,19 +43646,19 @@
       <c r="Z1" s="6"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="36" t="s">
-        <v>95</v>
+      <c r="A2" s="38" t="s">
+        <v>98</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>96</v>
+      <c r="B2" s="39" t="s">
+        <v>99</v>
       </c>
-      <c r="C2" s="38" t="s">
-        <v>96</v>
+      <c r="C2" s="40" t="s">
+        <v>99</v>
       </c>
-      <c r="D2" s="38" t="s">
-        <v>96</v>
+      <c r="D2" s="40" t="s">
+        <v>99</v>
       </c>
-      <c r="E2" s="39"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -43637,11 +43682,11 @@
       <c r="Z2" s="12"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="36" t="s">
-        <v>97</v>
+      <c r="A3" s="38" t="s">
+        <v>100</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>96</v>
+      <c r="B3" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -43669,11 +43714,11 @@
       <c r="Z3" s="13"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="36" t="s">
-        <v>98</v>
+      <c r="A4" s="38" t="s">
+        <v>101</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>96</v>
+      <c r="B4" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -43701,11 +43746,11 @@
       <c r="Z4" s="13"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="42" t="s">
         <v>99</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>96</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -43733,11 +43778,11 @@
       <c r="Z5" s="13"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="36" t="s">
-        <v>100</v>
+      <c r="A6" s="38" t="s">
+        <v>103</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>96</v>
+      <c r="B6" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -43765,14 +43810,14 @@
       <c r="Z6" s="13"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="36" t="s">
-        <v>101</v>
+      <c r="A7" s="38" t="s">
+        <v>104</v>
       </c>
-      <c r="B7" s="40" t="s">
-        <v>96</v>
+      <c r="B7" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>96</v>
+      <c r="C7" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="13"/>
@@ -43799,11 +43844,11 @@
       <c r="Z7" s="13"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="36" t="s">
-        <v>102</v>
+      <c r="A8" s="38" t="s">
+        <v>105</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>96</v>
+      <c r="B8" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -43831,11 +43876,11 @@
       <c r="Z8" s="13"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="36" t="s">
-        <v>103</v>
+      <c r="A9" s="38" t="s">
+        <v>106</v>
       </c>
-      <c r="B9" s="40" t="s">
-        <v>96</v>
+      <c r="B9" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -43863,11 +43908,11 @@
       <c r="Z9" s="13"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="36" t="s">
-        <v>104</v>
+      <c r="A10" s="38" t="s">
+        <v>107</v>
       </c>
-      <c r="B10" s="40" t="s">
-        <v>96</v>
+      <c r="B10" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -43895,11 +43940,11 @@
       <c r="Z10" s="13"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="36" t="s">
-        <v>105</v>
+      <c r="A11" s="38" t="s">
+        <v>108</v>
       </c>
-      <c r="B11" s="40" t="s">
-        <v>96</v>
+      <c r="B11" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -43927,17 +43972,17 @@
       <c r="Z11" s="13"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="36" t="s">
-        <v>106</v>
+      <c r="A12" s="38" t="s">
+        <v>109</v>
       </c>
-      <c r="B12" s="40" t="s">
-        <v>96</v>
+      <c r="B12" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C12" s="41" t="s">
-        <v>96</v>
+      <c r="C12" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D12" s="41" t="s">
-        <v>96</v>
+      <c r="D12" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -43963,11 +44008,11 @@
       <c r="Z12" s="13"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="36" t="s">
-        <v>107</v>
+      <c r="A13" s="38" t="s">
+        <v>110</v>
       </c>
-      <c r="B13" s="40" t="s">
-        <v>96</v>
+      <c r="B13" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -43995,14 +44040,14 @@
       <c r="Z13" s="13"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="36" t="s">
-        <v>108</v>
+      <c r="A14" s="38" t="s">
+        <v>111</v>
       </c>
-      <c r="B14" s="40" t="s">
-        <v>96</v>
+      <c r="B14" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C14" s="41" t="s">
-        <v>96</v>
+      <c r="C14" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="13"/>
@@ -44029,11 +44074,11 @@
       <c r="Z14" s="13"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="36" t="s">
-        <v>109</v>
+      <c r="A15" s="38" t="s">
+        <v>112</v>
       </c>
-      <c r="B15" s="40" t="s">
-        <v>96</v>
+      <c r="B15" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
@@ -44061,12 +44106,12 @@
       <c r="Z15" s="13"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="36" t="s">
-        <v>110</v>
+      <c r="A16" s="38" t="s">
+        <v>113</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="41" t="s">
-        <v>96</v>
+      <c r="B16" s="44"/>
+      <c r="C16" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="13"/>
@@ -44093,14 +44138,14 @@
       <c r="Z16" s="13"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="36" t="s">
-        <v>111</v>
+      <c r="A17" s="38" t="s">
+        <v>114</v>
       </c>
-      <c r="B17" s="40" t="s">
-        <v>96</v>
+      <c r="B17" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C17" s="41" t="s">
-        <v>96</v>
+      <c r="C17" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="13"/>
@@ -44127,11 +44172,11 @@
       <c r="Z17" s="13"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="36" t="s">
-        <v>112</v>
+      <c r="A18" s="38" t="s">
+        <v>115</v>
       </c>
-      <c r="B18" s="40" t="s">
-        <v>96</v>
+      <c r="B18" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -44159,15 +44204,15 @@
       <c r="Z18" s="13"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="36" t="s">
-        <v>113</v>
+      <c r="A19" s="38" t="s">
+        <v>116</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="41" t="s">
-        <v>96</v>
+      <c r="B19" s="44"/>
+      <c r="C19" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D19" s="41" t="s">
-        <v>96</v>
+      <c r="D19" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
@@ -44193,11 +44238,11 @@
       <c r="Z19" s="13"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="36" t="s">
-        <v>114</v>
+      <c r="A20" s="38" t="s">
+        <v>117</v>
       </c>
-      <c r="B20" s="40" t="s">
-        <v>96</v>
+      <c r="B20" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -44225,11 +44270,11 @@
       <c r="Z20" s="13"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="36" t="s">
-        <v>115</v>
+      <c r="A21" s="38" t="s">
+        <v>118</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>96</v>
+      <c r="B21" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -44257,11 +44302,11 @@
       <c r="Z21" s="13"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="36" t="s">
-        <v>116</v>
+      <c r="A22" s="38" t="s">
+        <v>119</v>
       </c>
-      <c r="B22" s="40" t="s">
-        <v>96</v>
+      <c r="B22" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -44289,11 +44334,11 @@
       <c r="Z22" s="13"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="36" t="s">
-        <v>117</v>
+      <c r="A23" s="38" t="s">
+        <v>120</v>
       </c>
-      <c r="B23" s="40" t="s">
-        <v>96</v>
+      <c r="B23" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -44321,11 +44366,11 @@
       <c r="Z23" s="13"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="36" t="s">
-        <v>118</v>
+      <c r="A24" s="38" t="s">
+        <v>121</v>
       </c>
-      <c r="B24" s="40" t="s">
-        <v>96</v>
+      <c r="B24" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -44353,11 +44398,11 @@
       <c r="Z24" s="13"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="36" t="s">
-        <v>119</v>
+      <c r="A25" s="38" t="s">
+        <v>122</v>
       </c>
-      <c r="B25" s="40" t="s">
-        <v>96</v>
+      <c r="B25" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -44385,11 +44430,11 @@
       <c r="Z25" s="13"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="36" t="s">
-        <v>120</v>
+      <c r="A26" s="38" t="s">
+        <v>123</v>
       </c>
-      <c r="B26" s="40" t="s">
-        <v>96</v>
+      <c r="B26" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -44417,11 +44462,11 @@
       <c r="Z26" s="13"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="36" t="s">
-        <v>121</v>
+      <c r="A27" s="38" t="s">
+        <v>124</v>
       </c>
-      <c r="B27" s="40" t="s">
-        <v>96</v>
+      <c r="B27" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -44449,17 +44494,17 @@
       <c r="Z27" s="13"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="36" t="s">
-        <v>122</v>
+      <c r="A28" s="38" t="s">
+        <v>125</v>
       </c>
-      <c r="B28" s="40" t="s">
-        <v>96</v>
+      <c r="B28" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>96</v>
+      <c r="C28" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D28" s="41" t="s">
-        <v>96</v>
+      <c r="D28" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
@@ -44485,11 +44530,11 @@
       <c r="Z28" s="13"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="36" t="s">
-        <v>123</v>
+      <c r="A29" s="38" t="s">
+        <v>126</v>
       </c>
-      <c r="B29" s="40" t="s">
-        <v>96</v>
+      <c r="B29" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -44517,11 +44562,11 @@
       <c r="Z29" s="13"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="36" t="s">
-        <v>124</v>
+      <c r="A30" s="38" t="s">
+        <v>127</v>
       </c>
-      <c r="B30" s="40" t="s">
-        <v>96</v>
+      <c r="B30" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -44549,11 +44594,11 @@
       <c r="Z30" s="13"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="36" t="s">
-        <v>125</v>
+      <c r="A31" s="38" t="s">
+        <v>128</v>
       </c>
-      <c r="B31" s="40" t="s">
-        <v>96</v>
+      <c r="B31" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -44581,11 +44626,11 @@
       <c r="Z31" s="13"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="36" t="s">
-        <v>126</v>
+      <c r="A32" s="38" t="s">
+        <v>129</v>
       </c>
-      <c r="B32" s="40" t="s">
-        <v>96</v>
+      <c r="B32" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -44613,11 +44658,11 @@
       <c r="Z32" s="13"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="36" t="s">
-        <v>127</v>
+      <c r="A33" s="38" t="s">
+        <v>130</v>
       </c>
-      <c r="B33" s="40" t="s">
-        <v>96</v>
+      <c r="B33" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -44645,11 +44690,11 @@
       <c r="Z33" s="13"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="36" t="s">
-        <v>128</v>
+      <c r="A34" s="38" t="s">
+        <v>131</v>
       </c>
-      <c r="B34" s="40" t="s">
-        <v>96</v>
+      <c r="B34" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
@@ -44677,11 +44722,11 @@
       <c r="Z34" s="13"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="36" t="s">
-        <v>129</v>
+      <c r="A35" s="38" t="s">
+        <v>132</v>
       </c>
-      <c r="B35" s="40" t="s">
-        <v>96</v>
+      <c r="B35" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -44709,11 +44754,11 @@
       <c r="Z35" s="13"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="36" t="s">
-        <v>130</v>
+      <c r="A36" s="38" t="s">
+        <v>133</v>
       </c>
-      <c r="B36" s="40" t="s">
-        <v>96</v>
+      <c r="B36" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
@@ -44741,17 +44786,17 @@
       <c r="Z36" s="13"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="36" t="s">
-        <v>131</v>
+      <c r="A37" s="38" t="s">
+        <v>134</v>
       </c>
-      <c r="B37" s="40" t="s">
-        <v>96</v>
+      <c r="B37" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C37" s="41" t="s">
-        <v>96</v>
+      <c r="C37" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D37" s="41" t="s">
-        <v>96</v>
+      <c r="D37" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
@@ -44777,11 +44822,11 @@
       <c r="Z37" s="13"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="36" t="s">
-        <v>132</v>
+      <c r="A38" s="38" t="s">
+        <v>135</v>
       </c>
-      <c r="B38" s="40" t="s">
-        <v>96</v>
+      <c r="B38" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
@@ -44809,11 +44854,11 @@
       <c r="Z38" s="13"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="36" t="s">
-        <v>133</v>
+      <c r="A39" s="38" t="s">
+        <v>136</v>
       </c>
-      <c r="B39" s="40" t="s">
-        <v>96</v>
+      <c r="B39" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -44841,11 +44886,11 @@
       <c r="Z39" s="13"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="36" t="s">
-        <v>134</v>
+      <c r="A40" s="38" t="s">
+        <v>137</v>
       </c>
-      <c r="B40" s="40" t="s">
-        <v>96</v>
+      <c r="B40" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
@@ -44873,14 +44918,14 @@
       <c r="Z40" s="13"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="36" t="s">
-        <v>135</v>
+      <c r="A41" s="38" t="s">
+        <v>138</v>
       </c>
-      <c r="B41" s="40" t="s">
-        <v>96</v>
+      <c r="B41" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C41" s="41" t="s">
-        <v>96</v>
+      <c r="C41" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="13"/>
@@ -44907,11 +44952,11 @@
       <c r="Z41" s="13"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="36" t="s">
-        <v>136</v>
+      <c r="A42" s="38" t="s">
+        <v>139</v>
       </c>
-      <c r="B42" s="40" t="s">
-        <v>96</v>
+      <c r="B42" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
@@ -44939,11 +44984,11 @@
       <c r="Z42" s="13"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="36" t="s">
-        <v>137</v>
+      <c r="A43" s="38" t="s">
+        <v>140</v>
       </c>
-      <c r="B43" s="40" t="s">
-        <v>96</v>
+      <c r="B43" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -44971,14 +45016,14 @@
       <c r="Z43" s="13"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="36" t="s">
-        <v>138</v>
+      <c r="A44" s="38" t="s">
+        <v>141</v>
       </c>
-      <c r="B44" s="40" t="s">
-        <v>96</v>
+      <c r="B44" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C44" s="41" t="s">
-        <v>96</v>
+      <c r="C44" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="13"/>
@@ -45005,11 +45050,11 @@
       <c r="Z44" s="13"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="36" t="s">
-        <v>139</v>
+      <c r="A45" s="38" t="s">
+        <v>142</v>
       </c>
-      <c r="B45" s="40" t="s">
-        <v>96</v>
+      <c r="B45" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
@@ -45037,14 +45082,14 @@
       <c r="Z45" s="13"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="36" t="s">
-        <v>140</v>
+      <c r="A46" s="38" t="s">
+        <v>143</v>
       </c>
-      <c r="B46" s="40" t="s">
-        <v>96</v>
+      <c r="B46" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C46" s="41" t="s">
-        <v>96</v>
+      <c r="C46" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="13"/>
@@ -45071,11 +45116,11 @@
       <c r="Z46" s="13"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="36" t="s">
-        <v>141</v>
+      <c r="A47" s="38" t="s">
+        <v>144</v>
       </c>
-      <c r="B47" s="40" t="s">
-        <v>96</v>
+      <c r="B47" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -45103,14 +45148,14 @@
       <c r="Z47" s="13"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="36" t="s">
-        <v>142</v>
+      <c r="A48" s="38" t="s">
+        <v>145</v>
       </c>
-      <c r="B48" s="40" t="s">
-        <v>96</v>
+      <c r="B48" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C48" s="41" t="s">
-        <v>96</v>
+      <c r="C48" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="13"/>
@@ -45137,11 +45182,11 @@
       <c r="Z48" s="13"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="36" t="s">
-        <v>143</v>
+      <c r="A49" s="38" t="s">
+        <v>146</v>
       </c>
-      <c r="B49" s="40" t="s">
-        <v>96</v>
+      <c r="B49" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C49" s="19"/>
       <c r="D49" s="19"/>
@@ -45169,11 +45214,11 @@
       <c r="Z49" s="13"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="36" t="s">
-        <v>144</v>
+      <c r="A50" s="38" t="s">
+        <v>147</v>
       </c>
-      <c r="B50" s="40" t="s">
-        <v>96</v>
+      <c r="B50" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="19"/>
@@ -45201,11 +45246,11 @@
       <c r="Z50" s="13"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="36" t="s">
-        <v>145</v>
+      <c r="A51" s="38" t="s">
+        <v>148</v>
       </c>
-      <c r="B51" s="40" t="s">
-        <v>96</v>
+      <c r="B51" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="19"/>
@@ -45233,11 +45278,11 @@
       <c r="Z51" s="13"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="36" t="s">
-        <v>146</v>
+      <c r="A52" s="38" t="s">
+        <v>149</v>
       </c>
-      <c r="B52" s="40" t="s">
-        <v>96</v>
+      <c r="B52" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="19"/>
@@ -45265,14 +45310,14 @@
       <c r="Z52" s="13"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="36" t="s">
-        <v>147</v>
+      <c r="A53" s="38" t="s">
+        <v>150</v>
       </c>
-      <c r="B53" s="40" t="s">
-        <v>96</v>
+      <c r="B53" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C53" s="41" t="s">
-        <v>96</v>
+      <c r="C53" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="13"/>
@@ -45299,14 +45344,14 @@
       <c r="Z53" s="13"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="36" t="s">
-        <v>148</v>
+      <c r="A54" s="38" t="s">
+        <v>151</v>
       </c>
-      <c r="B54" s="40" t="s">
-        <v>96</v>
+      <c r="B54" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C54" s="41" t="s">
-        <v>96</v>
+      <c r="C54" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D54" s="19"/>
       <c r="E54" s="13"/>
@@ -45333,11 +45378,11 @@
       <c r="Z54" s="13"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="36" t="s">
-        <v>149</v>
+      <c r="A55" s="38" t="s">
+        <v>152</v>
       </c>
-      <c r="B55" s="40" t="s">
-        <v>96</v>
+      <c r="B55" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
@@ -45365,11 +45410,11 @@
       <c r="Z55" s="13"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="36" t="s">
-        <v>150</v>
+      <c r="A56" s="38" t="s">
+        <v>153</v>
       </c>
-      <c r="B56" s="40" t="s">
-        <v>96</v>
+      <c r="B56" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
@@ -45397,14 +45442,14 @@
       <c r="Z56" s="13"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="36" t="s">
-        <v>151</v>
+      <c r="A57" s="38" t="s">
+        <v>154</v>
       </c>
-      <c r="B57" s="40" t="s">
-        <v>96</v>
+      <c r="B57" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C57" s="41" t="s">
-        <v>96</v>
+      <c r="C57" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="13"/>
@@ -45431,17 +45476,17 @@
       <c r="Z57" s="13"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="36" t="s">
-        <v>152</v>
+      <c r="A58" s="38" t="s">
+        <v>155</v>
       </c>
-      <c r="B58" s="40" t="s">
-        <v>96</v>
+      <c r="B58" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C58" s="41" t="s">
-        <v>96</v>
+      <c r="C58" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D58" s="41" t="s">
-        <v>96</v>
+      <c r="D58" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
@@ -45467,11 +45512,11 @@
       <c r="Z58" s="13"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="36" t="s">
-        <v>153</v>
+      <c r="A59" s="38" t="s">
+        <v>156</v>
       </c>
-      <c r="B59" s="40" t="s">
-        <v>96</v>
+      <c r="B59" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C59" s="19"/>
       <c r="D59" s="19"/>
@@ -45499,11 +45544,11 @@
       <c r="Z59" s="13"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="36" t="s">
-        <v>154</v>
+      <c r="A60" s="38" t="s">
+        <v>157</v>
       </c>
-      <c r="B60" s="40" t="s">
-        <v>96</v>
+      <c r="B60" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C60" s="19"/>
       <c r="D60" s="19"/>
@@ -45531,11 +45576,11 @@
       <c r="Z60" s="13"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="36" t="s">
-        <v>155</v>
+      <c r="A61" s="38" t="s">
+        <v>158</v>
       </c>
-      <c r="B61" s="40" t="s">
-        <v>96</v>
+      <c r="B61" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -45563,11 +45608,11 @@
       <c r="Z61" s="13"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="36" t="s">
-        <v>156</v>
+      <c r="A62" s="38" t="s">
+        <v>159</v>
       </c>
-      <c r="B62" s="40" t="s">
-        <v>96</v>
+      <c r="B62" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
@@ -45595,14 +45640,14 @@
       <c r="Z62" s="13"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="36" t="s">
-        <v>157</v>
+      <c r="A63" s="38" t="s">
+        <v>160</v>
       </c>
-      <c r="B63" s="40" t="s">
-        <v>96</v>
+      <c r="B63" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C63" s="41" t="s">
-        <v>96</v>
+      <c r="C63" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D63" s="19"/>
       <c r="E63" s="13"/>
@@ -45629,11 +45674,11 @@
       <c r="Z63" s="13"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="36" t="s">
-        <v>158</v>
+      <c r="A64" s="38" t="s">
+        <v>161</v>
       </c>
-      <c r="B64" s="40" t="s">
-        <v>96</v>
+      <c r="B64" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
@@ -45661,11 +45706,11 @@
       <c r="Z64" s="13"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="36" t="s">
-        <v>159</v>
+      <c r="A65" s="38" t="s">
+        <v>162</v>
       </c>
-      <c r="B65" s="40" t="s">
-        <v>96</v>
+      <c r="B65" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="19"/>
@@ -45693,11 +45738,11 @@
       <c r="Z65" s="13"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="36" t="s">
-        <v>160</v>
+      <c r="A66" s="38" t="s">
+        <v>163</v>
       </c>
-      <c r="B66" s="40" t="s">
-        <v>96</v>
+      <c r="B66" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C66" s="19"/>
       <c r="D66" s="19"/>
@@ -45725,14 +45770,14 @@
       <c r="Z66" s="13"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="36" t="s">
-        <v>161</v>
+      <c r="A67" s="38" t="s">
+        <v>164</v>
       </c>
-      <c r="B67" s="40" t="s">
-        <v>96</v>
+      <c r="B67" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C67" s="41" t="s">
-        <v>96</v>
+      <c r="C67" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D67" s="19"/>
       <c r="E67" s="13"/>
@@ -45759,11 +45804,11 @@
       <c r="Z67" s="13"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="36" t="s">
-        <v>162</v>
+      <c r="A68" s="38" t="s">
+        <v>165</v>
       </c>
-      <c r="B68" s="40" t="s">
-        <v>96</v>
+      <c r="B68" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="19"/>
@@ -45791,11 +45836,11 @@
       <c r="Z68" s="13"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="36" t="s">
-        <v>163</v>
+      <c r="A69" s="38" t="s">
+        <v>166</v>
       </c>
-      <c r="B69" s="40" t="s">
-        <v>96</v>
+      <c r="B69" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="19"/>
@@ -45823,11 +45868,11 @@
       <c r="Z69" s="13"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="36" t="s">
-        <v>164</v>
+      <c r="A70" s="38" t="s">
+        <v>167</v>
       </c>
-      <c r="B70" s="40" t="s">
-        <v>96</v>
+      <c r="B70" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="19"/>
@@ -45855,11 +45900,11 @@
       <c r="Z70" s="13"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="36" t="s">
-        <v>165</v>
+      <c r="A71" s="38" t="s">
+        <v>168</v>
       </c>
-      <c r="B71" s="40" t="s">
-        <v>96</v>
+      <c r="B71" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="19"/>
@@ -45887,17 +45932,17 @@
       <c r="Z71" s="13"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="36" t="s">
-        <v>166</v>
+      <c r="A72" s="38" t="s">
+        <v>169</v>
       </c>
-      <c r="B72" s="40" t="s">
-        <v>96</v>
+      <c r="B72" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C72" s="41" t="s">
-        <v>96</v>
+      <c r="C72" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D72" s="41" t="s">
-        <v>96</v>
+      <c r="D72" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E72" s="13"/>
       <c r="F72" s="13"/>
@@ -45923,14 +45968,14 @@
       <c r="Z72" s="13"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="36" t="s">
-        <v>167</v>
+      <c r="A73" s="38" t="s">
+        <v>170</v>
       </c>
-      <c r="B73" s="40" t="s">
-        <v>96</v>
+      <c r="B73" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C73" s="41" t="s">
-        <v>96</v>
+      <c r="C73" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D73" s="19"/>
       <c r="E73" s="13"/>
@@ -45957,11 +46002,11 @@
       <c r="Z73" s="13"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="36" t="s">
-        <v>168</v>
+      <c r="A74" s="38" t="s">
+        <v>171</v>
       </c>
-      <c r="B74" s="40" t="s">
-        <v>96</v>
+      <c r="B74" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C74" s="19"/>
       <c r="D74" s="19"/>
@@ -45989,11 +46034,11 @@
       <c r="Z74" s="13"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="36" t="s">
-        <v>169</v>
+      <c r="A75" s="38" t="s">
+        <v>172</v>
       </c>
-      <c r="B75" s="40" t="s">
-        <v>96</v>
+      <c r="B75" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="19"/>
@@ -46021,11 +46066,11 @@
       <c r="Z75" s="13"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="36" t="s">
-        <v>170</v>
+      <c r="A76" s="38" t="s">
+        <v>173</v>
       </c>
-      <c r="B76" s="40" t="s">
-        <v>96</v>
+      <c r="B76" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="19"/>
@@ -46053,17 +46098,17 @@
       <c r="Z76" s="13"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="36" t="s">
-        <v>171</v>
+      <c r="A77" s="38" t="s">
+        <v>174</v>
       </c>
-      <c r="B77" s="40" t="s">
-        <v>96</v>
+      <c r="B77" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C77" s="41" t="s">
-        <v>96</v>
+      <c r="C77" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D77" s="41" t="s">
-        <v>96</v>
+      <c r="D77" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E77" s="13"/>
       <c r="F77" s="13"/>
@@ -46089,14 +46134,14 @@
       <c r="Z77" s="13"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="36" t="s">
-        <v>172</v>
+      <c r="A78" s="38" t="s">
+        <v>175</v>
       </c>
-      <c r="B78" s="40" t="s">
-        <v>96</v>
+      <c r="B78" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C78" s="41" t="s">
-        <v>96</v>
+      <c r="C78" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D78" s="19"/>
       <c r="E78" s="13"/>
@@ -46123,11 +46168,11 @@
       <c r="Z78" s="13"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="36" t="s">
-        <v>173</v>
+      <c r="A79" s="38" t="s">
+        <v>176</v>
       </c>
-      <c r="B79" s="40" t="s">
-        <v>96</v>
+      <c r="B79" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C79" s="19"/>
       <c r="D79" s="19"/>
@@ -46155,14 +46200,14 @@
       <c r="Z79" s="13"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="36" t="s">
-        <v>174</v>
+      <c r="A80" s="38" t="s">
+        <v>177</v>
       </c>
-      <c r="B80" s="40" t="s">
-        <v>96</v>
+      <c r="B80" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C80" s="41" t="s">
-        <v>96</v>
+      <c r="C80" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D80" s="19"/>
       <c r="E80" s="13"/>
@@ -46189,11 +46234,11 @@
       <c r="Z80" s="13"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="36" t="s">
-        <v>175</v>
+      <c r="A81" s="38" t="s">
+        <v>178</v>
       </c>
-      <c r="B81" s="40" t="s">
-        <v>96</v>
+      <c r="B81" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C81" s="19"/>
       <c r="D81" s="19"/>
@@ -46221,11 +46266,11 @@
       <c r="Z81" s="13"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="36" t="s">
-        <v>176</v>
+      <c r="A82" s="38" t="s">
+        <v>179</v>
       </c>
-      <c r="B82" s="40" t="s">
-        <v>96</v>
+      <c r="B82" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C82" s="19"/>
       <c r="D82" s="19"/>
@@ -46253,11 +46298,11 @@
       <c r="Z82" s="13"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="36" t="s">
-        <v>177</v>
+      <c r="A83" s="38" t="s">
+        <v>180</v>
       </c>
-      <c r="B83" s="40" t="s">
-        <v>96</v>
+      <c r="B83" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C83" s="19"/>
       <c r="D83" s="19"/>
@@ -46285,11 +46330,11 @@
       <c r="Z83" s="13"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="36" t="s">
-        <v>178</v>
+      <c r="A84" s="38" t="s">
+        <v>181</v>
       </c>
-      <c r="B84" s="40" t="s">
-        <v>96</v>
+      <c r="B84" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C84" s="19"/>
       <c r="D84" s="19"/>
@@ -46317,11 +46362,11 @@
       <c r="Z84" s="13"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="36" t="s">
-        <v>179</v>
+      <c r="A85" s="38" t="s">
+        <v>182</v>
       </c>
-      <c r="B85" s="40" t="s">
-        <v>96</v>
+      <c r="B85" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C85" s="19"/>
       <c r="D85" s="19"/>
@@ -46349,11 +46394,11 @@
       <c r="Z85" s="13"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="36" t="s">
-        <v>180</v>
+      <c r="A86" s="38" t="s">
+        <v>183</v>
       </c>
-      <c r="B86" s="40" t="s">
-        <v>96</v>
+      <c r="B86" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C86" s="19"/>
       <c r="D86" s="19"/>
@@ -46381,11 +46426,11 @@
       <c r="Z86" s="13"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="36" t="s">
-        <v>181</v>
+      <c r="A87" s="38" t="s">
+        <v>184</v>
       </c>
-      <c r="B87" s="40" t="s">
-        <v>96</v>
+      <c r="B87" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C87" s="19"/>
       <c r="D87" s="19"/>
@@ -46413,14 +46458,14 @@
       <c r="Z87" s="13"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="36" t="s">
-        <v>182</v>
+      <c r="A88" s="38" t="s">
+        <v>185</v>
       </c>
-      <c r="B88" s="40" t="s">
-        <v>96</v>
+      <c r="B88" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C88" s="41" t="s">
-        <v>96</v>
+      <c r="C88" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D88" s="19"/>
       <c r="E88" s="13"/>
@@ -46447,11 +46492,11 @@
       <c r="Z88" s="13"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="36" t="s">
-        <v>183</v>
+      <c r="A89" s="38" t="s">
+        <v>186</v>
       </c>
-      <c r="B89" s="40" t="s">
-        <v>96</v>
+      <c r="B89" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C89" s="19"/>
       <c r="D89" s="19"/>
@@ -46479,11 +46524,11 @@
       <c r="Z89" s="13"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="36" t="s">
-        <v>184</v>
+      <c r="A90" s="38" t="s">
+        <v>187</v>
       </c>
-      <c r="B90" s="40" t="s">
-        <v>96</v>
+      <c r="B90" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C90" s="19"/>
       <c r="D90" s="19"/>
@@ -46511,17 +46556,17 @@
       <c r="Z90" s="13"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="36" t="s">
-        <v>185</v>
+      <c r="A91" s="38" t="s">
+        <v>188</v>
       </c>
-      <c r="B91" s="40" t="s">
-        <v>96</v>
+      <c r="B91" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C91" s="41" t="s">
-        <v>96</v>
+      <c r="C91" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D91" s="41" t="s">
-        <v>96</v>
+      <c r="D91" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E91" s="13"/>
       <c r="F91" s="13"/>
@@ -46547,14 +46592,14 @@
       <c r="Z91" s="13"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="36" t="s">
-        <v>186</v>
+      <c r="A92" s="38" t="s">
+        <v>189</v>
       </c>
-      <c r="B92" s="40" t="s">
-        <v>96</v>
+      <c r="B92" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C92" s="41" t="s">
-        <v>96</v>
+      <c r="C92" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D92" s="19"/>
       <c r="E92" s="13"/>
@@ -46581,15 +46626,15 @@
       <c r="Z92" s="13"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="36" t="s">
-        <v>187</v>
+      <c r="A93" s="38" t="s">
+        <v>190</v>
       </c>
-      <c r="B93" s="40" t="s">
-        <v>96</v>
+      <c r="B93" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C93" s="19"/>
-      <c r="D93" s="41" t="s">
-        <v>96</v>
+      <c r="D93" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E93" s="13"/>
       <c r="F93" s="13"/>
@@ -46615,14 +46660,14 @@
       <c r="Z93" s="13"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="36" t="s">
-        <v>188</v>
+      <c r="A94" s="38" t="s">
+        <v>191</v>
       </c>
-      <c r="B94" s="40" t="s">
-        <v>96</v>
+      <c r="B94" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C94" s="41" t="s">
-        <v>96</v>
+      <c r="C94" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D94" s="19"/>
       <c r="E94" s="13"/>
@@ -46649,14 +46694,14 @@
       <c r="Z94" s="13"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="36" t="s">
-        <v>189</v>
+      <c r="A95" s="38" t="s">
+        <v>192</v>
       </c>
-      <c r="B95" s="40" t="s">
-        <v>96</v>
+      <c r="B95" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C95" s="41" t="s">
-        <v>96</v>
+      <c r="C95" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D95" s="19"/>
       <c r="E95" s="13"/>
@@ -46683,11 +46728,11 @@
       <c r="Z95" s="13"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="36" t="s">
-        <v>190</v>
+      <c r="A96" s="38" t="s">
+        <v>193</v>
       </c>
-      <c r="B96" s="40" t="s">
-        <v>96</v>
+      <c r="B96" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C96" s="19"/>
       <c r="D96" s="19"/>
@@ -46715,11 +46760,11 @@
       <c r="Z96" s="13"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="36" t="s">
-        <v>191</v>
+      <c r="A97" s="38" t="s">
+        <v>194</v>
       </c>
-      <c r="B97" s="40" t="s">
-        <v>96</v>
+      <c r="B97" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C97" s="19"/>
       <c r="D97" s="19"/>
@@ -46747,11 +46792,11 @@
       <c r="Z97" s="13"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="36" t="s">
-        <v>192</v>
+      <c r="A98" s="38" t="s">
+        <v>195</v>
       </c>
-      <c r="B98" s="40" t="s">
-        <v>96</v>
+      <c r="B98" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C98" s="19"/>
       <c r="D98" s="19"/>
@@ -46779,11 +46824,11 @@
       <c r="Z98" s="13"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="36" t="s">
-        <v>193</v>
+      <c r="A99" s="38" t="s">
+        <v>196</v>
       </c>
-      <c r="B99" s="40" t="s">
-        <v>96</v>
+      <c r="B99" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C99" s="19"/>
       <c r="D99" s="19"/>
@@ -46811,11 +46856,11 @@
       <c r="Z99" s="13"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="36" t="s">
-        <v>194</v>
+      <c r="A100" s="38" t="s">
+        <v>197</v>
       </c>
-      <c r="B100" s="40" t="s">
-        <v>96</v>
+      <c r="B100" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C100" s="19"/>
       <c r="D100" s="19"/>
@@ -46843,17 +46888,17 @@
       <c r="Z100" s="13"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="36" t="s">
-        <v>195</v>
+      <c r="A101" s="38" t="s">
+        <v>198</v>
       </c>
-      <c r="B101" s="40" t="s">
-        <v>96</v>
+      <c r="B101" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C101" s="41" t="s">
-        <v>96</v>
+      <c r="C101" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D101" s="41" t="s">
-        <v>96</v>
+      <c r="D101" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
@@ -46879,11 +46924,11 @@
       <c r="Z101" s="13"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="36" t="s">
-        <v>196</v>
+      <c r="A102" s="38" t="s">
+        <v>199</v>
       </c>
-      <c r="B102" s="40" t="s">
-        <v>96</v>
+      <c r="B102" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C102" s="19"/>
       <c r="D102" s="19"/>
@@ -46911,15 +46956,15 @@
       <c r="Z102" s="13"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="36" t="s">
-        <v>197</v>
+      <c r="A103" s="38" t="s">
+        <v>200</v>
       </c>
-      <c r="B103" s="40" t="s">
-        <v>96</v>
+      <c r="B103" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C103" s="19"/>
-      <c r="D103" s="41" t="s">
-        <v>96</v>
+      <c r="D103" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E103" s="13"/>
       <c r="F103" s="13"/>
@@ -46945,14 +46990,14 @@
       <c r="Z103" s="13"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="36" t="s">
-        <v>198</v>
+      <c r="A104" s="38" t="s">
+        <v>201</v>
       </c>
-      <c r="B104" s="40" t="s">
-        <v>96</v>
+      <c r="B104" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C104" s="41" t="s">
-        <v>96</v>
+      <c r="C104" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D104" s="19"/>
       <c r="E104" s="13"/>
@@ -46979,11 +47024,11 @@
       <c r="Z104" s="13"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="36" t="s">
-        <v>199</v>
+      <c r="A105" s="38" t="s">
+        <v>202</v>
       </c>
-      <c r="B105" s="40" t="s">
-        <v>96</v>
+      <c r="B105" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C105" s="19"/>
       <c r="D105" s="19"/>
@@ -47011,11 +47056,11 @@
       <c r="Z105" s="13"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="36" t="s">
-        <v>200</v>
+      <c r="A106" s="38" t="s">
+        <v>203</v>
       </c>
-      <c r="B106" s="40" t="s">
-        <v>96</v>
+      <c r="B106" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C106" s="19"/>
       <c r="D106" s="19"/>
@@ -47043,11 +47088,11 @@
       <c r="Z106" s="13"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="36" t="s">
-        <v>201</v>
+      <c r="A107" s="38" t="s">
+        <v>204</v>
       </c>
-      <c r="B107" s="40" t="s">
-        <v>96</v>
+      <c r="B107" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C107" s="19"/>
       <c r="D107" s="19"/>
@@ -47075,11 +47120,11 @@
       <c r="Z107" s="13"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="36" t="s">
-        <v>202</v>
+      <c r="A108" s="38" t="s">
+        <v>205</v>
       </c>
-      <c r="B108" s="40" t="s">
-        <v>96</v>
+      <c r="B108" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C108" s="19"/>
       <c r="D108" s="19"/>
@@ -47107,11 +47152,11 @@
       <c r="Z108" s="13"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="36" t="s">
-        <v>203</v>
+      <c r="A109" s="38" t="s">
+        <v>206</v>
       </c>
-      <c r="B109" s="40" t="s">
-        <v>96</v>
+      <c r="B109" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C109" s="19"/>
       <c r="D109" s="19"/>
@@ -47139,11 +47184,11 @@
       <c r="Z109" s="13"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="36" t="s">
-        <v>204</v>
+      <c r="A110" s="38" t="s">
+        <v>207</v>
       </c>
-      <c r="B110" s="40" t="s">
-        <v>96</v>
+      <c r="B110" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C110" s="19"/>
       <c r="D110" s="19"/>
@@ -47171,11 +47216,11 @@
       <c r="Z110" s="13"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="36" t="s">
-        <v>205</v>
+      <c r="A111" s="38" t="s">
+        <v>208</v>
       </c>
-      <c r="B111" s="40" t="s">
-        <v>96</v>
+      <c r="B111" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C111" s="19"/>
       <c r="D111" s="19"/>
@@ -47203,11 +47248,11 @@
       <c r="Z111" s="13"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="43" t="s">
-        <v>206</v>
+      <c r="A112" s="45" t="s">
+        <v>209</v>
       </c>
-      <c r="B112" s="40" t="s">
-        <v>96</v>
+      <c r="B112" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C112" s="19"/>
       <c r="D112" s="19"/>
@@ -47235,14 +47280,14 @@
       <c r="Z112" s="13"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="36" t="s">
-        <v>207</v>
+      <c r="A113" s="38" t="s">
+        <v>210</v>
       </c>
-      <c r="B113" s="40" t="s">
-        <v>96</v>
+      <c r="B113" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C113" s="41" t="s">
-        <v>96</v>
+      <c r="C113" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D113" s="19"/>
       <c r="E113" s="13"/>
@@ -47269,14 +47314,14 @@
       <c r="Z113" s="13"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="36" t="s">
-        <v>208</v>
+      <c r="A114" s="38" t="s">
+        <v>211</v>
       </c>
-      <c r="B114" s="40" t="s">
-        <v>96</v>
+      <c r="B114" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C114" s="41" t="s">
-        <v>96</v>
+      <c r="C114" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D114" s="19"/>
       <c r="E114" s="13"/>
@@ -47303,11 +47348,11 @@
       <c r="Z114" s="13"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="36" t="s">
-        <v>209</v>
+      <c r="A115" s="38" t="s">
+        <v>212</v>
       </c>
-      <c r="B115" s="40" t="s">
-        <v>96</v>
+      <c r="B115" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C115" s="19"/>
       <c r="D115" s="19"/>
@@ -47335,14 +47380,14 @@
       <c r="Z115" s="13"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="36" t="s">
-        <v>210</v>
+      <c r="A116" s="38" t="s">
+        <v>213</v>
       </c>
-      <c r="B116" s="40" t="s">
-        <v>96</v>
+      <c r="B116" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C116" s="41" t="s">
-        <v>96</v>
+      <c r="C116" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D116" s="19"/>
       <c r="E116" s="13"/>
@@ -47369,11 +47414,11 @@
       <c r="Z116" s="13"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="36" t="s">
-        <v>211</v>
+      <c r="A117" s="38" t="s">
+        <v>214</v>
       </c>
-      <c r="B117" s="40" t="s">
-        <v>96</v>
+      <c r="B117" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C117" s="19"/>
       <c r="D117" s="19"/>
@@ -47401,11 +47446,11 @@
       <c r="Z117" s="13"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="36" t="s">
-        <v>212</v>
+      <c r="A118" s="38" t="s">
+        <v>215</v>
       </c>
-      <c r="B118" s="40" t="s">
-        <v>96</v>
+      <c r="B118" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C118" s="19"/>
       <c r="D118" s="19"/>
@@ -47433,11 +47478,11 @@
       <c r="Z118" s="13"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="36" t="s">
-        <v>213</v>
+      <c r="A119" s="38" t="s">
+        <v>216</v>
       </c>
-      <c r="B119" s="40" t="s">
-        <v>96</v>
+      <c r="B119" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C119" s="19"/>
       <c r="D119" s="19"/>
@@ -47465,14 +47510,14 @@
       <c r="Z119" s="13"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="36" t="s">
-        <v>214</v>
+      <c r="A120" s="38" t="s">
+        <v>217</v>
       </c>
-      <c r="B120" s="40" t="s">
-        <v>96</v>
+      <c r="B120" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C120" s="41" t="s">
-        <v>96</v>
+      <c r="C120" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D120" s="19"/>
       <c r="E120" s="13"/>
@@ -47499,14 +47544,14 @@
       <c r="Z120" s="13"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="36" t="s">
-        <v>215</v>
+      <c r="A121" s="38" t="s">
+        <v>218</v>
       </c>
-      <c r="B121" s="40" t="s">
-        <v>96</v>
+      <c r="B121" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C121" s="41" t="s">
-        <v>96</v>
+      <c r="C121" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D121" s="19"/>
       <c r="E121" s="13"/>
@@ -47533,17 +47578,17 @@
       <c r="Z121" s="13"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="36" t="s">
-        <v>216</v>
+      <c r="A122" s="38" t="s">
+        <v>219</v>
       </c>
-      <c r="B122" s="40" t="s">
-        <v>96</v>
+      <c r="B122" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C122" s="41" t="s">
-        <v>96</v>
+      <c r="C122" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D122" s="41" t="s">
-        <v>96</v>
+      <c r="D122" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E122" s="13"/>
       <c r="F122" s="13"/>
@@ -47569,11 +47614,11 @@
       <c r="Z122" s="13"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="36" t="s">
-        <v>217</v>
+      <c r="A123" s="38" t="s">
+        <v>220</v>
       </c>
-      <c r="B123" s="40" t="s">
-        <v>96</v>
+      <c r="B123" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C123" s="19"/>
       <c r="D123" s="19"/>
@@ -47601,11 +47646,11 @@
       <c r="Z123" s="13"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="36" t="s">
-        <v>218</v>
+      <c r="A124" s="38" t="s">
+        <v>221</v>
       </c>
-      <c r="B124" s="40" t="s">
-        <v>96</v>
+      <c r="B124" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C124" s="19"/>
       <c r="D124" s="19"/>
@@ -47633,11 +47678,11 @@
       <c r="Z124" s="13"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="36" t="s">
-        <v>219</v>
+      <c r="A125" s="38" t="s">
+        <v>222</v>
       </c>
-      <c r="B125" s="40" t="s">
-        <v>96</v>
+      <c r="B125" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C125" s="19"/>
       <c r="D125" s="19"/>
@@ -47665,11 +47710,11 @@
       <c r="Z125" s="13"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="36" t="s">
-        <v>220</v>
+      <c r="A126" s="38" t="s">
+        <v>223</v>
       </c>
-      <c r="B126" s="40" t="s">
-        <v>96</v>
+      <c r="B126" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C126" s="19"/>
       <c r="D126" s="19"/>
@@ -47697,11 +47742,11 @@
       <c r="Z126" s="13"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="36" t="s">
-        <v>221</v>
+      <c r="A127" s="38" t="s">
+        <v>224</v>
       </c>
-      <c r="B127" s="40" t="s">
-        <v>96</v>
+      <c r="B127" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C127" s="19"/>
       <c r="D127" s="19"/>
@@ -47729,14 +47774,14 @@
       <c r="Z127" s="13"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="36" t="s">
-        <v>222</v>
+      <c r="A128" s="38" t="s">
+        <v>225</v>
       </c>
-      <c r="B128" s="40" t="s">
-        <v>96</v>
+      <c r="B128" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C128" s="41" t="s">
-        <v>96</v>
+      <c r="C128" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D128" s="19"/>
       <c r="E128" s="13"/>
@@ -47763,14 +47808,14 @@
       <c r="Z128" s="13"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="36" t="s">
-        <v>223</v>
+      <c r="A129" s="38" t="s">
+        <v>226</v>
       </c>
-      <c r="B129" s="40" t="s">
-        <v>96</v>
+      <c r="B129" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C129" s="41" t="s">
-        <v>96</v>
+      <c r="C129" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D129" s="19"/>
       <c r="E129" s="13"/>
@@ -47797,11 +47842,11 @@
       <c r="Z129" s="13"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="36" t="s">
-        <v>224</v>
+      <c r="A130" s="38" t="s">
+        <v>227</v>
       </c>
-      <c r="B130" s="40" t="s">
-        <v>96</v>
+      <c r="B130" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C130" s="19"/>
       <c r="D130" s="19"/>
@@ -47829,11 +47874,11 @@
       <c r="Z130" s="13"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="36" t="s">
-        <v>225</v>
+      <c r="A131" s="38" t="s">
+        <v>228</v>
       </c>
-      <c r="B131" s="40" t="s">
-        <v>96</v>
+      <c r="B131" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C131" s="19"/>
       <c r="D131" s="19"/>
@@ -47861,14 +47906,14 @@
       <c r="Z131" s="13"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="36" t="s">
-        <v>226</v>
+      <c r="A132" s="38" t="s">
+        <v>229</v>
       </c>
-      <c r="B132" s="40" t="s">
-        <v>96</v>
+      <c r="B132" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C132" s="41" t="s">
-        <v>96</v>
+      <c r="C132" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D132" s="19"/>
       <c r="E132" s="13"/>
@@ -47895,14 +47940,14 @@
       <c r="Z132" s="13"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="36" t="s">
-        <v>227</v>
+      <c r="A133" s="38" t="s">
+        <v>230</v>
       </c>
-      <c r="B133" s="40" t="s">
-        <v>96</v>
+      <c r="B133" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C133" s="41" t="s">
-        <v>96</v>
+      <c r="C133" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D133" s="19"/>
       <c r="E133" s="13"/>
@@ -47929,11 +47974,11 @@
       <c r="Z133" s="13"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="36" t="s">
-        <v>228</v>
+      <c r="A134" s="38" t="s">
+        <v>231</v>
       </c>
-      <c r="B134" s="40" t="s">
-        <v>96</v>
+      <c r="B134" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C134" s="19"/>
       <c r="D134" s="19"/>
@@ -47961,11 +48006,11 @@
       <c r="Z134" s="13"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="36" t="s">
-        <v>229</v>
+      <c r="A135" s="38" t="s">
+        <v>232</v>
       </c>
-      <c r="B135" s="40" t="s">
-        <v>96</v>
+      <c r="B135" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C135" s="19"/>
       <c r="D135" s="19"/>
@@ -47993,17 +48038,17 @@
       <c r="Z135" s="13"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="36" t="s">
-        <v>230</v>
+      <c r="A136" s="38" t="s">
+        <v>233</v>
       </c>
-      <c r="B136" s="40" t="s">
-        <v>96</v>
+      <c r="B136" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C136" s="41" t="s">
-        <v>96</v>
+      <c r="C136" s="43" t="s">
+        <v>99</v>
       </c>
-      <c r="D136" s="41" t="s">
-        <v>96</v>
+      <c r="D136" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="E136" s="13"/>
       <c r="F136" s="13"/>
@@ -48029,11 +48074,11 @@
       <c r="Z136" s="13"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="36" t="s">
-        <v>231</v>
+      <c r="A137" s="38" t="s">
+        <v>234</v>
       </c>
-      <c r="B137" s="40" t="s">
-        <v>96</v>
+      <c r="B137" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C137" s="19"/>
       <c r="D137" s="19"/>
@@ -48061,11 +48106,11 @@
       <c r="Z137" s="13"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="36" t="s">
-        <v>232</v>
+      <c r="A138" s="38" t="s">
+        <v>235</v>
       </c>
-      <c r="B138" s="40" t="s">
-        <v>96</v>
+      <c r="B138" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C138" s="19"/>
       <c r="D138" s="19"/>
@@ -48093,11 +48138,11 @@
       <c r="Z138" s="13"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="36" t="s">
-        <v>233</v>
+      <c r="A139" s="38" t="s">
+        <v>236</v>
       </c>
-      <c r="B139" s="40" t="s">
-        <v>96</v>
+      <c r="B139" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C139" s="19"/>
       <c r="D139" s="19"/>
@@ -48125,11 +48170,11 @@
       <c r="Z139" s="13"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="36" t="s">
-        <v>234</v>
+      <c r="A140" s="38" t="s">
+        <v>237</v>
       </c>
-      <c r="B140" s="40" t="s">
-        <v>96</v>
+      <c r="B140" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C140" s="19"/>
       <c r="D140" s="19"/>
@@ -48157,11 +48202,11 @@
       <c r="Z140" s="13"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="36" t="s">
-        <v>235</v>
+      <c r="A141" s="38" t="s">
+        <v>238</v>
       </c>
-      <c r="B141" s="40" t="s">
-        <v>96</v>
+      <c r="B141" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C141" s="19"/>
       <c r="D141" s="19"/>
@@ -48189,11 +48234,11 @@
       <c r="Z141" s="13"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="36" t="s">
-        <v>236</v>
+      <c r="A142" s="38" t="s">
+        <v>239</v>
       </c>
-      <c r="B142" s="40" t="s">
-        <v>96</v>
+      <c r="B142" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C142" s="19"/>
       <c r="D142" s="19"/>
@@ -48221,11 +48266,11 @@
       <c r="Z142" s="13"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="36" t="s">
-        <v>237</v>
+      <c r="A143" s="38" t="s">
+        <v>240</v>
       </c>
-      <c r="B143" s="40" t="s">
-        <v>96</v>
+      <c r="B143" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C143" s="19"/>
       <c r="D143" s="19"/>
@@ -48253,14 +48298,14 @@
       <c r="Z143" s="13"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="43" t="s">
-        <v>238</v>
+      <c r="A144" s="45" t="s">
+        <v>241</v>
       </c>
-      <c r="B144" s="40" t="s">
-        <v>96</v>
+      <c r="B144" s="42" t="s">
+        <v>99</v>
       </c>
-      <c r="C144" s="41" t="s">
-        <v>96</v>
+      <c r="C144" s="43" t="s">
+        <v>99</v>
       </c>
       <c r="D144" s="19"/>
       <c r="E144" s="13"/>
@@ -48287,11 +48332,11 @@
       <c r="Z144" s="13"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="44" t="s">
-        <v>239</v>
+      <c r="A145" s="46" t="s">
+        <v>242</v>
       </c>
-      <c r="B145" s="40" t="s">
-        <v>96</v>
+      <c r="B145" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C145" s="19"/>
       <c r="D145" s="19"/>

</xml_diff>

<commit_message>
🐞 Transmission fixes (#1404)
Parent issue: https://github.com/sequentech/meta/issues/5046
</commit_message>
<xml_diff>
--- a/packages/windmill/external-bin/janitor/17-12-2024-parameters-reports.xlsx
+++ b/packages/windmill/external-bin/janitor/17-12-2024-parameters-reports.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="293">
   <si>
     <t>name</t>
   </si>
@@ -44936,7 +44936,9 @@
       <c r="B35" s="44" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="35"/>
+      <c r="C35" s="44" t="s">
+        <v>101</v>
+      </c>
       <c r="D35" s="35"/>
       <c r="E35" s="44" t="s">
         <v>101</v>

</xml_diff>